<commit_message>
Changed via hole size to pass eurocircuits inner anular ring Fixed supplier information for capacitors
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="165">
   <si>
     <t>Item #</t>
   </si>
@@ -49,10 +49,10 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>17/10/2017</t>
-  </si>
-  <si>
-    <t>17:12:07</t>
+    <t>18/10/2017</t>
+  </si>
+  <si>
+    <t>12:40:18</t>
   </si>
   <si>
     <t>20</t>
@@ -265,9 +265,6 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 0.1uF 10% X7R</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 25volts 18pF 2% C0G</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 33pF 5% C0G</t>
   </si>
   <si>
@@ -364,7 +361,7 @@
     <t>06035C104KAT2A</t>
   </si>
   <si>
-    <t>02013A180GAT2A</t>
+    <t>06031A180GAT2A</t>
   </si>
   <si>
     <t>06035A330JAT2A</t>
@@ -439,7 +436,7 @@
     <t>581-06035C104KAT2A</t>
   </si>
   <si>
-    <t>581-02013A180GAT2A</t>
+    <t>581-06031A180GAT2A</t>
   </si>
   <si>
     <t>581-06035A330J</t>
@@ -1317,37 +1314,37 @@
         <v>81</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>8</v>
@@ -1378,25 +1375,25 @@
         <v>82</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" s="10">
-        <v>448529</v>
+        <v>444509</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O2" s="10">
         <v>3</v>
@@ -1439,28 +1436,28 @@
         <v>74</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L3" s="10">
-        <v>33130</v>
+        <v>10288</v>
       </c>
       <c r="M3" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O3" s="10">
         <v>2</v>
@@ -1473,11 +1470,11 @@
         <v>40</v>
       </c>
       <c r="R3" s="30">
-        <v>0.28599999999999998</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="S3" s="30">
         <f t="shared" ref="S3:S22" si="2">R3*Q3</f>
-        <v>11.44</v>
+        <v>10.760000000000002</v>
       </c>
       <c r="T3" s="50">
         <f t="shared" ref="T3:T22" si="3">ROW(T3) - ROW($A$1)</f>
@@ -1503,28 +1500,28 @@
         <v>74</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L4" s="10">
         <v>85002</v>
       </c>
       <c r="M4" s="58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O4" s="10">
         <v>2</v>
@@ -1567,28 +1564,28 @@
         <v>74</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="10">
         <v>160</v>
       </c>
       <c r="M5" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N5" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O5" s="10">
         <v>2</v>
@@ -1634,25 +1631,25 @@
         <v>75</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L6" s="10">
         <v>0</v>
       </c>
       <c r="M6" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N6" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O6" s="10">
         <v>1</v>
@@ -1695,28 +1692,28 @@
         <v>75</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L7" s="10">
         <v>0</v>
       </c>
       <c r="M7" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N7" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O7" s="10">
         <v>1</v>
@@ -1759,28 +1756,28 @@
         <v>75</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J8" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L8" s="10">
-        <v>218238</v>
+        <v>218163</v>
       </c>
       <c r="M8" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O8" s="10">
         <v>1</v>
@@ -1823,28 +1820,28 @@
         <v>76</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" s="57" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L9" s="10">
         <v>8268</v>
       </c>
       <c r="M9" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N9" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O9" s="10">
         <v>1</v>
@@ -1887,28 +1884,28 @@
         <v>75</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" s="10">
         <v>18358</v>
       </c>
       <c r="M10" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N10" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O10" s="10">
         <v>1</v>
@@ -1951,28 +1948,28 @@
         <v>77</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I11" s="57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N11" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O11" s="10">
         <v>1</v>
@@ -2015,28 +2012,28 @@
         <v>78</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N12" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O12" s="10">
         <v>5</v>
@@ -2079,28 +2076,28 @@
         <v>78</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
       </c>
       <c r="M13" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N13" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O13" s="10">
         <v>1</v>
@@ -2143,28 +2140,28 @@
         <v>78</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L14" s="10">
-        <v>1346281</v>
+        <v>1274838</v>
       </c>
       <c r="M14" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N14" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O14" s="10">
         <v>1</v>
@@ -2207,28 +2204,28 @@
         <v>78</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L15" s="10">
         <v>38932</v>
       </c>
       <c r="M15" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N15" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O15" s="10">
         <v>1</v>
@@ -2271,28 +2268,28 @@
         <v>78</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H16" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L16" s="10">
-        <v>7715</v>
+        <v>12715</v>
       </c>
       <c r="M16" s="58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O16" s="10">
         <v>1</v>
@@ -2335,28 +2332,28 @@
         <v>78</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J17" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L17" s="10">
         <v>0</v>
       </c>
       <c r="M17" s="58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O17" s="10">
         <v>2</v>
@@ -2399,28 +2396,28 @@
         <v>78</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L18" s="10">
-        <v>149925</v>
+        <v>149825</v>
       </c>
       <c r="M18" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N18" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O18" s="10">
         <v>2</v>
@@ -2463,28 +2460,28 @@
         <v>79</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19" s="57" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L19" s="10">
         <v>23022</v>
       </c>
       <c r="M19" s="58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N19" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O19" s="10">
         <v>2</v>
@@ -2527,28 +2524,28 @@
         <v>75</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I20" s="57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L20" s="10">
         <v>1605</v>
       </c>
       <c r="M20" s="58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N20" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O20" s="10">
         <v>1</v>
@@ -2591,28 +2588,28 @@
         <v>75</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I21" s="57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L21" s="10">
         <v>14229</v>
       </c>
       <c r="M21" s="58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N21" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O21" s="10">
         <v>1</v>
@@ -2655,28 +2652,28 @@
         <v>80</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I22" s="57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L22" s="10">
-        <v>4207</v>
+        <v>2682</v>
       </c>
       <c r="M22" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N22" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O22" s="10">
         <v>1</v>
@@ -2746,7 +2743,7 @@
       <c r="L24" s="14"/>
       <c r="M24" s="35">
         <f ca="1">NOW()</f>
-        <v>43025.716827662036</v>
+        <v>43026.528066087965</v>
       </c>
       <c r="N24" s="41"/>
       <c r="O24" s="15"/>
@@ -2757,11 +2754,11 @@
       </c>
       <c r="S24" s="37">
         <f>SUM(S2:S22)</f>
-        <v>183.09999999999997</v>
+        <v>182.42</v>
       </c>
       <c r="T24" s="45">
         <f>(SUM(S2:S22))/P25</f>
-        <v>9.1549999999999976</v>
+        <v>9.1209999999999987</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2809,7 +2806,7 @@
     <hyperlink ref="H21" r:id="rId20" tooltip="Component" display="'Texas Instruments"/>
     <hyperlink ref="H22" r:id="rId21" tooltip="Component" display="'TXC Corporation"/>
     <hyperlink ref="I2" r:id="rId22" tooltip="Manufacturer" display="'06035C104KAT2A"/>
-    <hyperlink ref="I3" r:id="rId23" tooltip="Manufacturer" display="'02013A180GAT2A"/>
+    <hyperlink ref="I3" r:id="rId23" tooltip="Manufacturer" display="'06031A180GAT2A"/>
     <hyperlink ref="I4" r:id="rId24" tooltip="Manufacturer" display="'06035A330JAT2A"/>
     <hyperlink ref="I5" r:id="rId25" tooltip="Manufacturer" display="'GCM188R71C105KA64D"/>
     <hyperlink ref="I6" r:id="rId26" tooltip="Manufacturer" display="'LS L29K-G1J2-1-Z"/>
@@ -2830,7 +2827,7 @@
     <hyperlink ref="I21" r:id="rId41" tooltip="Manufacturer" display="'TPS78233DDCR"/>
     <hyperlink ref="I22" r:id="rId42" tooltip="Manufacturer" display="'8Z-12.000MAAJ-T"/>
     <hyperlink ref="M2" r:id="rId43" tooltip="Supplier" display="'581-06035C104KAT2A"/>
-    <hyperlink ref="M3" r:id="rId44" tooltip="Supplier" display="'581-02013A180GAT2A"/>
+    <hyperlink ref="M3" r:id="rId44" tooltip="Supplier" display="'581-06031A180GAT2A"/>
     <hyperlink ref="M4" r:id="rId45" tooltip="Supplier" display="'581-06035A330J"/>
     <hyperlink ref="M5" r:id="rId46" tooltip="Supplier" display="'81-GCM188R71C105K64D"/>
     <hyperlink ref="M6" r:id="rId47" tooltip="Supplier" display="'720-LSL29K-G1J2-1-Z"/>

</xml_diff>

<commit_message>
run outjobs, make all deliverables, run replacer, update manually timestamped gerberfiles.zip, update eurocircuits (was waiting our reply)
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="PurchaseList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -49,10 +49,10 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>18/10/2017</t>
-  </si>
-  <si>
-    <t>12:40:18</t>
+    <t>27/10/2017</t>
+  </si>
+  <si>
+    <t>16:11:44</t>
   </si>
   <si>
     <t>20</t>
@@ -193,10 +193,7 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>0603_cap</t>
-  </si>
-  <si>
-    <t>0603_CAP</t>
+    <t>0603_CAP_SMALL</t>
   </si>
   <si>
     <t>0603_LED_RED</t>
@@ -208,16 +205,16 @@
     <t>0603_LED_BLU</t>
   </si>
   <si>
-    <t>0603_DIODE-CDSU101A</t>
-  </si>
-  <si>
-    <t>USB-MINI-B-HIR-UX60A-MB-5ST</t>
+    <t>0603_DIODE-NSR20F30</t>
+  </si>
+  <si>
+    <t>USB-MINI-B-HIR-UX60A-MB-5ST-SMALL</t>
   </si>
   <si>
     <t>SOT323/SC70-3_SMALL</t>
   </si>
   <si>
-    <t>0603_res</t>
+    <t>0603_res_SMALL</t>
   </si>
   <si>
     <t>BUTTON_4.7x3.5mm</t>
@@ -244,7 +241,7 @@
     <t/>
   </si>
   <si>
-    <t>DIODE</t>
+    <t>SCHOTTKY DIODE 0603</t>
   </si>
   <si>
     <t>POWER MOSFET-P SOT23</t>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>1.3</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00"/>
@@ -1305,34 +1305,34 @@
         <v>58</v>
       </c>
       <c r="E1" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="G1" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>162</v>
@@ -1369,31 +1369,31 @@
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L2" s="10">
-        <v>444509</v>
+        <v>323877</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O2" s="10">
         <v>3</v>
@@ -1433,31 +1433,31 @@
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>75</v>
-      </c>
       <c r="H3" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L3" s="10">
         <v>10288</v>
       </c>
       <c r="M3" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O3" s="10">
         <v>2</v>
@@ -1497,31 +1497,31 @@
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L4" s="10">
-        <v>85002</v>
+        <v>84802</v>
       </c>
       <c r="M4" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O4" s="10">
         <v>2</v>
@@ -1557,35 +1557,35 @@
         <v>40</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L5" s="10">
+        <v>718765</v>
+      </c>
+      <c r="M5" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="N5" s="43" t="s">
         <v>160</v>
-      </c>
-      <c r="M5" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="N5" s="43" t="s">
-        <v>161</v>
       </c>
       <c r="O5" s="10">
         <v>2</v>
@@ -1598,11 +1598,11 @@
         <v>40</v>
       </c>
       <c r="R5" s="30">
-        <v>0.17799999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="S5" s="30">
         <f t="shared" ref="S5" si="5">R5*Q5</f>
-        <v>7.1199999999999992</v>
+        <v>7.4399999999999995</v>
       </c>
       <c r="T5" s="50">
         <f t="shared" si="3"/>
@@ -1621,35 +1621,35 @@
         <v>41</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L6" s="10">
         <v>0</v>
       </c>
       <c r="M6" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N6" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O6" s="10">
         <v>1</v>
@@ -1685,35 +1685,35 @@
         <v>42</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L7" s="10">
         <v>0</v>
       </c>
       <c r="M7" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N7" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O7" s="10">
         <v>1</v>
@@ -1749,35 +1749,35 @@
         <v>43</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J8" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L8" s="10">
-        <v>218163</v>
+        <v>214586</v>
       </c>
       <c r="M8" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O8" s="10">
         <v>1</v>
@@ -1813,32 +1813,32 @@
         <v>44</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="57" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L9" s="10">
-        <v>8268</v>
+        <v>6910</v>
       </c>
       <c r="M9" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N9" s="43" t="s">
         <v>161</v>
@@ -1851,14 +1851,14 @@
       </c>
       <c r="Q9" s="49">
         <f t="shared" ref="Q9" si="8">ROUNDUP(P9*N9,0)</f>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="R9" s="30">
         <v>0.32400000000000001</v>
       </c>
       <c r="S9" s="30">
         <f t="shared" ref="S9" si="9">R9*Q9</f>
-        <v>6.48</v>
+        <v>8.4239999999999995</v>
       </c>
       <c r="T9" s="50">
         <f t="shared" si="3"/>
@@ -1877,35 +1877,35 @@
         <v>45</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L10" s="10">
-        <v>18358</v>
+        <v>18067</v>
       </c>
       <c r="M10" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N10" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O10" s="10">
         <v>1</v>
@@ -1941,35 +1941,35 @@
         <v>46</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I11" s="57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N11" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O11" s="10">
         <v>1</v>
@@ -2005,35 +2005,35 @@
         <v>47</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N12" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O12" s="10">
         <v>5</v>
@@ -2069,35 +2069,35 @@
         <v>48</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
       </c>
       <c r="M13" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N13" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O13" s="10">
         <v>1</v>
@@ -2133,35 +2133,35 @@
         <v>49</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14" s="10">
-        <v>1274838</v>
+        <v>1022780</v>
       </c>
       <c r="M14" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N14" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O14" s="10">
         <v>1</v>
@@ -2197,35 +2197,35 @@
         <v>50</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L15" s="10">
-        <v>38932</v>
+        <v>38924</v>
       </c>
       <c r="M15" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N15" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O15" s="10">
         <v>1</v>
@@ -2261,35 +2261,35 @@
         <v>51</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L16" s="10">
-        <v>12715</v>
+        <v>12252</v>
       </c>
       <c r="M16" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O16" s="10">
         <v>1</v>
@@ -2325,35 +2325,35 @@
         <v>52</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J17" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L17" s="10">
-        <v>0</v>
+        <v>27987</v>
       </c>
       <c r="M17" s="58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O17" s="10">
         <v>2</v>
@@ -2389,35 +2389,35 @@
         <v>53</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I18" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L18" s="10">
-        <v>149825</v>
+        <v>216663</v>
       </c>
       <c r="M18" s="58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N18" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O18" s="10">
         <v>2</v>
@@ -2453,35 +2453,35 @@
         <v>54</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" s="57" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L19" s="10">
         <v>23022</v>
       </c>
       <c r="M19" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N19" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O19" s="10">
         <v>2</v>
@@ -2517,35 +2517,35 @@
         <v>55</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20" s="57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L20" s="10">
-        <v>1605</v>
+        <v>5015</v>
       </c>
       <c r="M20" s="58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N20" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O20" s="10">
         <v>1</v>
@@ -2581,35 +2581,35 @@
         <v>56</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I21" s="57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L21" s="10">
-        <v>14229</v>
+        <v>17939</v>
       </c>
       <c r="M21" s="58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N21" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O21" s="10">
         <v>1</v>
@@ -2645,35 +2645,35 @@
         <v>57</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I22" s="57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L22" s="10">
-        <v>2682</v>
+        <v>2377</v>
       </c>
       <c r="M22" s="58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N22" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O22" s="10">
         <v>1</v>
@@ -2743,7 +2743,7 @@
       <c r="L24" s="14"/>
       <c r="M24" s="35">
         <f ca="1">NOW()</f>
-        <v>43026.528066087965</v>
+        <v>43035.674917129632</v>
       </c>
       <c r="N24" s="41"/>
       <c r="O24" s="15"/>
@@ -2754,11 +2754,11 @@
       </c>
       <c r="S24" s="37">
         <f>SUM(S2:S22)</f>
-        <v>182.42</v>
+        <v>184.68399999999997</v>
       </c>
       <c r="T24" s="45">
         <f>(SUM(S2:S22))/P25</f>
-        <v>9.1209999999999987</v>
+        <v>9.2341999999999977</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
red and green led supplier info change due to availablity. run  BOM outjob
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="167">
   <si>
     <t>Item #</t>
   </si>
@@ -49,10 +49,10 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>27/10/2017</t>
-  </si>
-  <si>
-    <t>16:11:44</t>
+    <t>31/10/2017</t>
+  </si>
+  <si>
+    <t>09:26:15</t>
   </si>
   <si>
     <t>20</t>
@@ -268,7 +268,10 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 1.0uF 16volts X7R 10%</t>
   </si>
   <si>
-    <t>Standard LEDs - SMD Green, 570nm 10mcd, 2mA</t>
+    <t>Standard LEDs - SMD Super Red, 633nm 180mcd, 20mA</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD GREEN WATER CLEAR</t>
   </si>
   <si>
     <t>Standard LEDs - SMD Blue, 470nm 45mcd, 5mA</t>
@@ -328,6 +331,9 @@
     <t>OSRAM Opto Semiconductors</t>
   </si>
   <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
     <t>ON Semiconductor</t>
   </si>
   <si>
@@ -367,10 +373,10 @@
     <t>GCM188R71C105KA64D</t>
   </si>
   <si>
-    <t>LS L29K-G1J2-1-Z</t>
-  </si>
-  <si>
-    <t>LG L29K-F2J1-24-Z</t>
+    <t>LS Q976-NR-1</t>
+  </si>
+  <si>
+    <t>APT1608SGC</t>
   </si>
   <si>
     <t>LB Q39G-L2OO-35-1</t>
@@ -442,10 +448,10 @@
     <t>81-GCM188R71C105K64D</t>
   </si>
   <si>
-    <t>720-LSL29K-G1J2-1-Z</t>
-  </si>
-  <si>
-    <t>720-LGL29KF2J124Z</t>
+    <t>720-LSQ976-NR-1</t>
+  </si>
+  <si>
+    <t>604-APT1608SGC</t>
   </si>
   <si>
     <t>720-LBQ39GL2N2351</t>
@@ -1314,37 +1320,37 @@
         <v>80</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>8</v>
@@ -1375,25 +1381,25 @@
         <v>81</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L2" s="10">
-        <v>323877</v>
+        <v>310846</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O2" s="10">
         <v>3</v>
@@ -1439,25 +1445,25 @@
         <v>74</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I3" s="57" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L3" s="10">
-        <v>10288</v>
+        <v>10285</v>
       </c>
       <c r="M3" s="58" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O3" s="10">
         <v>2</v>
@@ -1503,25 +1509,25 @@
         <v>82</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L4" s="10">
-        <v>84802</v>
+        <v>84787</v>
       </c>
       <c r="M4" s="58" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O4" s="10">
         <v>2</v>
@@ -1567,25 +1573,25 @@
         <v>83</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L5" s="10">
-        <v>718765</v>
+        <v>718242</v>
       </c>
       <c r="M5" s="58" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N5" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O5" s="10">
         <v>2</v>
@@ -1628,28 +1634,28 @@
         <v>74</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L6" s="10">
-        <v>0</v>
+        <v>378706</v>
       </c>
       <c r="M6" s="58" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="N6" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O6" s="10">
         <v>1</v>
@@ -1662,11 +1668,11 @@
         <v>20</v>
       </c>
       <c r="R6" s="30">
-        <v>0.19500000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="S6" s="30">
         <f>R6*Q6</f>
-        <v>3.9000000000000004</v>
+        <v>2.92</v>
       </c>
       <c r="T6" s="50">
         <f>ROW(T6) - ROW($A$1)</f>
@@ -1692,28 +1698,28 @@
         <v>74</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L7" s="10">
-        <v>0</v>
+        <v>131423</v>
       </c>
       <c r="M7" s="58" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N7" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O7" s="10">
         <v>1</v>
@@ -1726,11 +1732,11 @@
         <v>20</v>
       </c>
       <c r="R7" s="30">
-        <v>0.16900000000000001</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="S7" s="30">
         <f t="shared" ref="S7" si="7">R7*Q7</f>
-        <v>3.3800000000000003</v>
+        <v>1.42</v>
       </c>
       <c r="T7" s="50">
         <f t="shared" si="3"/>
@@ -1756,28 +1762,28 @@
         <v>74</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J8" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L8" s="10">
-        <v>214586</v>
+        <v>190552</v>
       </c>
       <c r="M8" s="58" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O8" s="10">
         <v>1</v>
@@ -1820,28 +1826,28 @@
         <v>75</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I9" s="57" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L9" s="10">
         <v>6910</v>
       </c>
       <c r="M9" s="58" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N9" s="43" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="O9" s="10">
         <v>1</v>
@@ -1884,28 +1890,28 @@
         <v>74</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L10" s="10">
-        <v>18067</v>
+        <v>18014</v>
       </c>
       <c r="M10" s="58" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N10" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O10" s="10">
         <v>1</v>
@@ -1948,28 +1954,28 @@
         <v>76</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I11" s="57" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="M11" s="58" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N11" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O11" s="10">
         <v>1</v>
@@ -2012,28 +2018,28 @@
         <v>77</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N12" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O12" s="10">
         <v>5</v>
@@ -2076,28 +2082,28 @@
         <v>77</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
       </c>
       <c r="M13" s="58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="N13" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O13" s="10">
         <v>1</v>
@@ -2140,28 +2146,28 @@
         <v>77</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L14" s="10">
-        <v>1022780</v>
+        <v>987320</v>
       </c>
       <c r="M14" s="58" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N14" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O14" s="10">
         <v>1</v>
@@ -2204,28 +2210,28 @@
         <v>77</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L15" s="10">
         <v>38924</v>
       </c>
       <c r="M15" s="58" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N15" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O15" s="10">
         <v>1</v>
@@ -2268,28 +2274,28 @@
         <v>77</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H16" s="57" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L16" s="10">
         <v>12252</v>
       </c>
       <c r="M16" s="58" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N16" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O16" s="10">
         <v>1</v>
@@ -2332,28 +2338,28 @@
         <v>77</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J17" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L17" s="10">
-        <v>27987</v>
+        <v>25904</v>
       </c>
       <c r="M17" s="58" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="N17" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O17" s="10">
         <v>2</v>
@@ -2396,28 +2402,28 @@
         <v>77</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I18" s="57" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L18" s="10">
-        <v>216663</v>
+        <v>216662</v>
       </c>
       <c r="M18" s="58" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N18" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O18" s="10">
         <v>2</v>
@@ -2460,28 +2466,28 @@
         <v>78</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I19" s="57" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L19" s="10">
         <v>23022</v>
       </c>
       <c r="M19" s="58" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N19" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O19" s="10">
         <v>2</v>
@@ -2524,28 +2530,28 @@
         <v>74</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I20" s="57" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J20" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L20" s="10">
         <v>5015</v>
       </c>
       <c r="M20" s="58" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N20" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O20" s="10">
         <v>1</v>
@@ -2588,28 +2594,28 @@
         <v>74</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I21" s="57" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L21" s="10">
-        <v>17939</v>
+        <v>23179</v>
       </c>
       <c r="M21" s="58" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="N21" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O21" s="10">
         <v>1</v>
@@ -2652,28 +2658,28 @@
         <v>79</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I22" s="57" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L22" s="10">
-        <v>2377</v>
+        <v>2369</v>
       </c>
       <c r="M22" s="58" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N22" s="43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O22" s="10">
         <v>1</v>
@@ -2743,7 +2749,7 @@
       <c r="L24" s="14"/>
       <c r="M24" s="35">
         <f ca="1">NOW()</f>
-        <v>43035.674917129632</v>
+        <v>43039.393317476854</v>
       </c>
       <c r="N24" s="41"/>
       <c r="O24" s="15"/>
@@ -2754,11 +2760,11 @@
       </c>
       <c r="S24" s="37">
         <f>SUM(S2:S22)</f>
-        <v>184.68399999999997</v>
+        <v>181.74399999999997</v>
       </c>
       <c r="T24" s="45">
         <f>(SUM(S2:S22))/P25</f>
-        <v>9.2341999999999977</v>
+        <v>9.0871999999999993</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2789,7 +2795,7 @@
     <hyperlink ref="H4" r:id="rId3" tooltip="Component" display="'AVX"/>
     <hyperlink ref="H5" r:id="rId4" tooltip="Component" display="'Murata Electronics"/>
     <hyperlink ref="H6" r:id="rId5" tooltip="Component" display="'OSRAM Opto Semiconductors"/>
-    <hyperlink ref="H7" r:id="rId6" tooltip="Component" display="'OSRAM Opto Semiconductors"/>
+    <hyperlink ref="H7" r:id="rId6" tooltip="Component" display="'Kingbright"/>
     <hyperlink ref="H8" r:id="rId7" tooltip="Component" display="'OSRAM Opto Semiconductors"/>
     <hyperlink ref="H9" r:id="rId8" tooltip="Component" display="'ON Semiconductor"/>
     <hyperlink ref="H10" r:id="rId9" tooltip="Component" display="'Hirose Connector"/>
@@ -2809,8 +2815,8 @@
     <hyperlink ref="I3" r:id="rId23" tooltip="Manufacturer" display="'06031A180GAT2A"/>
     <hyperlink ref="I4" r:id="rId24" tooltip="Manufacturer" display="'06035A330JAT2A"/>
     <hyperlink ref="I5" r:id="rId25" tooltip="Manufacturer" display="'GCM188R71C105KA64D"/>
-    <hyperlink ref="I6" r:id="rId26" tooltip="Manufacturer" display="'LS L29K-G1J2-1-Z"/>
-    <hyperlink ref="I7" r:id="rId27" tooltip="Manufacturer" display="'LG L29K-F2J1-24-Z"/>
+    <hyperlink ref="I6" r:id="rId26" tooltip="Manufacturer" display="'LS Q976-NR-1"/>
+    <hyperlink ref="I7" r:id="rId27" tooltip="Manufacturer" display="'APT1608SGC"/>
     <hyperlink ref="I8" r:id="rId28" tooltip="Manufacturer" display="'LB Q39G-L2OO-35-1"/>
     <hyperlink ref="I9" r:id="rId29" tooltip="Manufacturer" display="'NSR20F30NXT5G"/>
     <hyperlink ref="I10" r:id="rId30" tooltip="Manufacturer" display="'UX60A-MB-5ST"/>
@@ -2830,8 +2836,8 @@
     <hyperlink ref="M3" r:id="rId44" tooltip="Supplier" display="'581-06031A180GAT2A"/>
     <hyperlink ref="M4" r:id="rId45" tooltip="Supplier" display="'581-06035A330J"/>
     <hyperlink ref="M5" r:id="rId46" tooltip="Supplier" display="'81-GCM188R71C105K64D"/>
-    <hyperlink ref="M6" r:id="rId47" tooltip="Supplier" display="'720-LSL29K-G1J2-1-Z"/>
-    <hyperlink ref="M7" r:id="rId48" tooltip="Supplier" display="'720-LGL29KF2J124Z"/>
+    <hyperlink ref="M6" r:id="rId47" tooltip="Supplier" display="'720-LSQ976-NR-1"/>
+    <hyperlink ref="M7" r:id="rId48" tooltip="Supplier" display="'604-APT1608SGC"/>
     <hyperlink ref="M8" r:id="rId49" tooltip="Supplier" display="'720-LBQ39GL2N2351"/>
     <hyperlink ref="M9" r:id="rId50" tooltip="Supplier" display="'863-NSR20F30NXT5G"/>
     <hyperlink ref="M10" r:id="rId51" tooltip="Supplier" display="'798-UX60A-MB-5ST"/>

</xml_diff>

<commit_message>
revert to old smaller size, new aurocircuits basket number: B2205801
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\n-blocks\n-dap\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5A951D3-B09B-4091-A96E-22F4886AD1D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{261A2B59-1474-423D-A746-F0EA66FCE9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="141">
   <si>
     <t>Item #</t>
   </si>
@@ -63,7 +63,7 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>16:31</t>
+    <t>17:43</t>
   </si>
   <si>
     <t>20</t>
@@ -135,9 +135,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
   </si>
   <si>
     <t>12MHz</t>
-  </si>
-  <si>
-    <t>N-5</t>
   </si>
   <si>
     <t>Footprint</t>
@@ -1206,7 +1200,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
@@ -1240,46 +1234,46 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>8</v>
@@ -1297,31 +1291,31 @@
         <v>14</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H2" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="J2" s="10">
-        <v>1903646</v>
+        <v>1903578</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L2" s="42">
         <v>1</v>
@@ -1350,38 +1344,38 @@
     </row>
     <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A23" si="0">ROW(A3) - ROW($A$1)</f>
+        <f t="shared" ref="A3:A22" si="0">ROW(A3) - ROW($A$1)</f>
         <v>2</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H3" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J3" s="10">
         <v>5890</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L3" s="42">
         <v>1</v>
@@ -1393,18 +1387,18 @@
         <v>200</v>
       </c>
       <c r="O3" s="47">
-        <f t="shared" ref="O3:O23" si="1">ROUNDUP(N3*L3,0)</f>
+        <f t="shared" ref="O3:O22" si="1">ROUNDUP(N3*L3,0)</f>
         <v>200</v>
       </c>
       <c r="P3" s="30">
         <v>0.16994999999999999</v>
       </c>
       <c r="Q3" s="30">
-        <f t="shared" ref="Q3:Q23" si="2">P3*O3</f>
+        <f t="shared" ref="Q3:Q22" si="2">P3*O3</f>
         <v>33.989999999999995</v>
       </c>
       <c r="R3" s="48">
-        <f t="shared" ref="R3:R23" si="3">ROW(R3) - ROW($A$1)</f>
+        <f t="shared" ref="R3:R22" si="3">ROW(R3) - ROW($A$1)</f>
         <v>2</v>
       </c>
     </row>
@@ -1417,31 +1411,31 @@
         <v>16</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H4" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J4" s="10">
         <v>99945</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L4" s="42">
         <v>1</v>
@@ -1477,31 +1471,31 @@
         <v>17</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J5" s="10">
         <v>237124</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L5" s="42">
         <v>1</v>
@@ -1537,29 +1531,29 @@
         <v>18</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H6" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J6" s="10">
         <v>68800</v>
       </c>
       <c r="K6" s="46" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L6" s="42">
         <v>1</v>
@@ -1595,29 +1589,29 @@
         <v>19</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="51" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H7" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="J7" s="10">
-        <v>43738</v>
+        <v>43490</v>
       </c>
       <c r="K7" s="46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L7" s="42">
         <v>1</v>
@@ -1653,29 +1647,29 @@
         <v>20</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H8" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J8" s="10">
         <v>58555</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L8" s="42">
         <v>1</v>
@@ -1711,31 +1705,31 @@
         <v>21</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G9" s="51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J9" s="10">
         <v>115642</v>
       </c>
       <c r="K9" s="46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L9" s="42">
         <v>1.3</v>
@@ -1771,29 +1765,29 @@
         <v>22</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="51" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G10" s="51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H10" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J10" s="10">
         <v>22003</v>
       </c>
       <c r="K10" s="46" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L10" s="42">
         <v>1</v>
@@ -1829,31 +1823,31 @@
         <v>23</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G11" s="51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H11" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J11" s="10">
         <v>97994</v>
       </c>
       <c r="K11" s="46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L11" s="42">
         <v>1</v>
@@ -1889,31 +1883,31 @@
         <v>24</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G12" s="51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H12" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J12" s="10">
         <v>1924459</v>
       </c>
       <c r="K12" s="46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L12" s="42">
         <v>1</v>
@@ -1949,31 +1943,31 @@
         <v>25</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H13" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J13" s="10">
         <v>23930</v>
       </c>
       <c r="K13" s="46" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L13" s="42">
         <v>1</v>
@@ -2009,31 +2003,31 @@
         <v>26</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H14" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J14" s="10">
         <v>231704</v>
       </c>
       <c r="K14" s="46" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L14" s="42">
         <v>1</v>
@@ -2069,31 +2063,31 @@
         <v>27</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H15" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J15" s="10">
         <v>54524</v>
       </c>
       <c r="K15" s="46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L15" s="42">
         <v>1</v>
@@ -2129,31 +2123,31 @@
         <v>28</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H16" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J16" s="10">
         <v>70706</v>
       </c>
       <c r="K16" s="46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L16" s="42">
         <v>1</v>
@@ -2189,31 +2183,31 @@
         <v>29</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G17" s="51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H17" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="J17" s="10">
-        <v>4399591</v>
+        <v>4399293</v>
       </c>
       <c r="K17" s="46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L17" s="42">
         <v>1</v>
@@ -2249,31 +2243,31 @@
         <v>30</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H18" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J18" s="10">
         <v>19360</v>
       </c>
       <c r="K18" s="46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L18" s="42">
         <v>1</v>
@@ -2309,31 +2303,31 @@
         <v>31</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G19" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J19" s="10">
         <v>15015</v>
       </c>
       <c r="K19" s="46" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L19" s="42">
         <v>1</v>
@@ -2345,14 +2339,14 @@
         <v>200</v>
       </c>
       <c r="O19" s="47">
-        <f t="shared" ref="O19:O23" si="18">ROUNDUP(N19*L19,0)</f>
+        <f t="shared" ref="O19:O22" si="18">ROUNDUP(N19*L19,0)</f>
         <v>200</v>
       </c>
       <c r="P19" s="30">
         <v>0.48826999999999998</v>
       </c>
       <c r="Q19" s="30">
-        <f t="shared" ref="Q19:Q23" si="19">P19*O19</f>
+        <f t="shared" ref="Q19:Q22" si="19">P19*O19</f>
         <v>97.653999999999996</v>
       </c>
       <c r="R19" s="48">
@@ -2369,29 +2363,29 @@
         <v>32</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G20" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H20" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J20" s="10">
         <v>843</v>
       </c>
       <c r="K20" s="46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L20" s="42">
         <v>1</v>
@@ -2427,29 +2421,29 @@
         <v>33</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G21" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H21" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J21" s="10">
         <v>27461</v>
       </c>
       <c r="K21" s="46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L21" s="42">
         <v>1</v>
@@ -2485,31 +2479,31 @@
         <v>34</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G22" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="52" t="s">
+      <c r="I22" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="J22" s="10">
         <v>959</v>
       </c>
       <c r="K22" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L22" s="42">
         <v>1</v>
@@ -2536,124 +2530,84 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="10">
-        <v>1</v>
-      </c>
-      <c r="N23" s="44"/>
-      <c r="O23" s="47">
-        <f t="shared" ref="O23" si="22">ROUNDUP(N23*L23,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30">
-        <f t="shared" ref="Q23" si="23">P23*O23</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="48">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
+    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
+    <row r="24" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="I24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="14"/>
+      <c r="K24" s="34">
+        <f ca="1">NOW()</f>
+        <v>43843.738721527778</v>
+      </c>
+      <c r="L24" s="40"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="36">
+        <f>SUM(Q2:Q22)</f>
+        <v>752.05489999999998</v>
+      </c>
+      <c r="R24" s="50">
+        <f>Q24/N25</f>
+        <v>37.602744999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="16"/>
-      <c r="I25" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J25" s="14"/>
-      <c r="K25" s="34">
-        <f ca="1">NOW()</f>
-        <v>43843.688709374997</v>
-      </c>
-      <c r="L25" s="40"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q25" s="36">
-        <f>SUM(Q2:Q23)</f>
-        <v>752.05489999999998</v>
-      </c>
-      <c r="R25" s="50">
-        <f>Q25/N26</f>
-        <v>37.602744999999999</v>
+    <row r="25" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K25" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="41"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="39"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="R25" s="43" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K26" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="41"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="O26" s="39"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="R26" s="43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="N27" s="49"/>
+    <row r="26" spans="1:18" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="49"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
all resitors & capacitors from 0603 to 0402, new eurocircuits basket B2206781
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\n-blocks\n-dap\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{261A2B59-1474-423D-A746-F0EA66FCE9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD0FDED8-F30A-4328-A0F5-7F410E4AA455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="144">
   <si>
     <t>Item #</t>
   </si>
@@ -63,7 +63,7 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>17:43</t>
+    <t>11:49</t>
   </si>
   <si>
     <t>20</t>
@@ -204,7 +204,7 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>0603_CAP_SMALL</t>
+    <t>0402_CAP</t>
   </si>
   <si>
     <t>0603_LED_RED</t>
@@ -225,7 +225,10 @@
     <t>SOT323/SC70-3_SMALL</t>
   </si>
   <si>
-    <t>0603_res_SMALL</t>
+    <t>0402_res</t>
+  </si>
+  <si>
+    <t>0402_RES</t>
   </si>
   <si>
     <t>BUTTON_4.7x3.5mm</t>
@@ -264,10 +267,13 @@
     <t>Manufacturer 1</t>
   </si>
   <si>
-    <t>Kyocera AVX</t>
-  </si>
-  <si>
-    <t>Murata</t>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>Walsin Technologies</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
   </si>
   <si>
     <t>Osram Opto</t>
@@ -285,12 +291,15 @@
     <t>Diodes</t>
   </si>
   <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductors</t>
+  </si>
+  <si>
     <t>Panasonic</t>
   </si>
   <si>
-    <t>Susumu</t>
-  </si>
-  <si>
     <t>NXP Semiconductors</t>
   </si>
   <si>
@@ -303,16 +312,16 @@
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
-    <t>06035C104KAT2A</t>
-  </si>
-  <si>
-    <t>06031A180GAT2A</t>
-  </si>
-  <si>
-    <t>06035A330JAT2A/4K</t>
-  </si>
-  <si>
-    <t>GCM188R71C105KA64D</t>
+    <t>885012105016</t>
+  </si>
+  <si>
+    <t>0402N180F500CT</t>
+  </si>
+  <si>
+    <t>885012005058</t>
+  </si>
+  <si>
+    <t>JMK105BJ105KP-F</t>
   </si>
   <si>
     <t>LSQ976-NR-1</t>
@@ -330,25 +339,25 @@
     <t>BSS84W-7-F</t>
   </si>
   <si>
-    <t>ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t>RR0816P-681-D</t>
-  </si>
-  <si>
-    <t>ERJ3EKF4700V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF33R0V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1501V</t>
-  </si>
-  <si>
-    <t>ERJ-3GEY0R00V</t>
-  </si>
-  <si>
-    <t>ERJ-3GEYJ183V</t>
+    <t>CRCW040210K0FKEDC</t>
+  </si>
+  <si>
+    <t>CRCW0402680RFKEDC</t>
+  </si>
+  <si>
+    <t>CRCW0402470RFKEDC</t>
+  </si>
+  <si>
+    <t>CRCW040233R0FKEDC</t>
+  </si>
+  <si>
+    <t>CRCW04021K50FKEDC</t>
+  </si>
+  <si>
+    <t>CRCW04020000Z0EDC</t>
+  </si>
+  <si>
+    <t>CRCW040218K0FKED</t>
   </si>
   <si>
     <t>LPC11U35FHI33/501,</t>
@@ -378,16 +387,16 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
-    <t>581-06035C104KAT2A</t>
-  </si>
-  <si>
-    <t>581-06031A180GAT2A</t>
-  </si>
-  <si>
-    <t>581-06035A330J</t>
-  </si>
-  <si>
-    <t>81-GCM188R71C105K64D</t>
+    <t>710-885012105016</t>
+  </si>
+  <si>
+    <t>791-0402N180F500CT</t>
+  </si>
+  <si>
+    <t>710-885012005058</t>
+  </si>
+  <si>
+    <t>963-JMK105BJ105KP-F</t>
   </si>
   <si>
     <t>720-LSQ976-NR-1</t>
@@ -408,25 +417,25 @@
     <t>621-BSS84W-F</t>
   </si>
   <si>
-    <t>667-ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t>754-RR0816P-681D</t>
-  </si>
-  <si>
-    <t>667-ERJ-3EKF4700V</t>
-  </si>
-  <si>
-    <t>667-ERJ-3EKF33R0V</t>
-  </si>
-  <si>
-    <t>667-ERJ-3EKF1501V</t>
-  </si>
-  <si>
-    <t>667-ERJ-3GEY0R00V</t>
-  </si>
-  <si>
-    <t>667-ERJ-3GEYJ183V</t>
+    <t>71-CRCW040210K0FKEDC</t>
+  </si>
+  <si>
+    <t>71-CRCW0402680RFKEDC</t>
+  </si>
+  <si>
+    <t>71-CRCW0402470RFKEDC</t>
+  </si>
+  <si>
+    <t>71-CRCW040233R0FKEDC</t>
+  </si>
+  <si>
+    <t>71-CRCW04021K50FKEDC</t>
+  </si>
+  <si>
+    <t>71-CRCW04020000Z0EDC</t>
+  </si>
+  <si>
+    <t>71-CRCW0402-18K-E3</t>
   </si>
   <si>
     <t>667-EVQ-P2202M</t>
@@ -1240,40 +1249,40 @@
         <v>57</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>8</v>
@@ -1297,25 +1306,25 @@
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H2" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J2" s="10">
-        <v>1903578</v>
+        <v>40996</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="L2" s="42">
         <v>1</v>
@@ -1331,18 +1340,18 @@
         <v>300</v>
       </c>
       <c r="P2" s="30">
-        <v>4.2259999999999999E-2</v>
+        <v>1.8849999999999999E-2</v>
       </c>
       <c r="Q2" s="30">
         <f>P2*O2</f>
-        <v>12.677999999999999</v>
+        <v>5.6549999999999994</v>
       </c>
       <c r="R2" s="48">
         <f>ROW(R2) - ROW($A$1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A22" si="0">ROW(A3) - ROW($A$1)</f>
         <v>2</v>
@@ -1357,25 +1366,25 @@
         <v>58</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J3" s="10">
-        <v>5890</v>
+        <v>5900</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="L3" s="42">
         <v>1</v>
@@ -1391,11 +1400,11 @@
         <v>200</v>
       </c>
       <c r="P3" s="30">
-        <v>0.16994999999999999</v>
+        <v>3.5909999999999997E-2</v>
       </c>
       <c r="Q3" s="30">
         <f t="shared" ref="Q3:Q22" si="2">P3*O3</f>
-        <v>33.989999999999995</v>
+        <v>7.1819999999999995</v>
       </c>
       <c r="R3" s="48">
         <f t="shared" ref="R3:R22" si="3">ROW(R3) - ROW($A$1)</f>
@@ -1417,25 +1426,25 @@
         <v>58</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J4" s="10">
-        <v>99945</v>
+        <v>34052</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L4" s="42">
         <v>1</v>
@@ -1451,11 +1460,11 @@
         <v>200</v>
       </c>
       <c r="P4" s="30">
-        <v>2.7879999999999999E-2</v>
+        <v>1.257E-2</v>
       </c>
       <c r="Q4" s="30">
         <f>P4*O4</f>
-        <v>5.5759999999999996</v>
+        <v>2.5139999999999998</v>
       </c>
       <c r="R4" s="48">
         <f>ROW(R4) - ROW($A$1)</f>
@@ -1477,25 +1486,25 @@
         <v>58</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J5" s="10">
-        <v>237124</v>
+        <v>25442</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="L5" s="42">
         <v>1</v>
@@ -1511,11 +1520,11 @@
         <v>200</v>
       </c>
       <c r="P5" s="30">
-        <v>8.9020000000000002E-2</v>
+        <v>2.8729999999999999E-2</v>
       </c>
       <c r="Q5" s="30">
         <f t="shared" ref="Q5" si="5">P5*O5</f>
-        <v>17.804000000000002</v>
+        <v>5.7459999999999996</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="3"/>
@@ -1538,22 +1547,22 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="51" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H6" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J6" s="10">
-        <v>68800</v>
+        <v>68575</v>
       </c>
       <c r="K6" s="46" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="L6" s="42">
         <v>1</v>
@@ -1569,11 +1578,11 @@
         <v>100</v>
       </c>
       <c r="P6" s="30">
-        <v>6.8339999999999998E-2</v>
+        <v>6.8220000000000003E-2</v>
       </c>
       <c r="Q6" s="30">
         <f>P6*O6</f>
-        <v>6.8339999999999996</v>
+        <v>6.8220000000000001</v>
       </c>
       <c r="R6" s="48">
         <f>ROW(R6) - ROW($A$1)</f>
@@ -1596,22 +1605,22 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="51" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J7" s="10">
         <v>43490</v>
       </c>
       <c r="K7" s="46" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="L7" s="42">
         <v>1</v>
@@ -1627,11 +1636,11 @@
         <v>100</v>
       </c>
       <c r="P7" s="30">
-        <v>5.0360000000000002E-2</v>
+        <v>5.0270000000000002E-2</v>
       </c>
       <c r="Q7" s="30">
         <f t="shared" ref="Q7:Q9" si="7">P7*O7</f>
-        <v>5.0360000000000005</v>
+        <v>5.0270000000000001</v>
       </c>
       <c r="R7" s="48">
         <f t="shared" si="3"/>
@@ -1654,22 +1663,22 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="51" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J8" s="10">
-        <v>58555</v>
+        <v>58553</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L8" s="42">
         <v>1</v>
@@ -1685,11 +1694,11 @@
         <v>100</v>
       </c>
       <c r="P8" s="30">
-        <v>0.10879999999999999</v>
+        <v>0.10861999999999999</v>
       </c>
       <c r="Q8" s="30">
         <f>P8*O8</f>
-        <v>10.879999999999999</v>
+        <v>10.862</v>
       </c>
       <c r="R8" s="48">
         <f>ROW(R8) - ROW($A$1)</f>
@@ -1711,25 +1720,25 @@
         <v>62</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G9" s="51" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J9" s="10">
         <v>115642</v>
       </c>
       <c r="K9" s="46" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L9" s="42">
         <v>1.3</v>
@@ -1745,11 +1754,11 @@
         <v>130</v>
       </c>
       <c r="P9" s="30">
-        <v>0.18612999999999999</v>
+        <v>0.18582000000000001</v>
       </c>
       <c r="Q9" s="30">
         <f t="shared" ref="Q9" si="9">P9*O9</f>
-        <v>24.196899999999999</v>
+        <v>24.156600000000001</v>
       </c>
       <c r="R9" s="48">
         <f t="shared" si="3"/>
@@ -1772,22 +1781,22 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="51" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G10" s="51" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J10" s="10">
-        <v>22003</v>
+        <v>21568</v>
       </c>
       <c r="K10" s="46" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="L10" s="42">
         <v>1</v>
@@ -1803,11 +1812,11 @@
         <v>100</v>
       </c>
       <c r="P10" s="30">
-        <v>0.61414999999999997</v>
+        <v>0.61312</v>
       </c>
       <c r="Q10" s="30">
         <f>P10*O10</f>
-        <v>61.414999999999999</v>
+        <v>61.311999999999998</v>
       </c>
       <c r="R10" s="48">
         <f>ROW(R10) - ROW($A$1)</f>
@@ -1829,25 +1838,25 @@
         <v>64</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G11" s="51" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H11" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J11" s="10">
-        <v>97994</v>
+        <v>97989</v>
       </c>
       <c r="K11" s="46" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L11" s="42">
         <v>1</v>
@@ -1863,11 +1872,11 @@
         <v>100</v>
       </c>
       <c r="P11" s="30">
-        <v>0.10251</v>
+        <v>0.10234</v>
       </c>
       <c r="Q11" s="30">
         <f t="shared" ref="Q11:Q17" si="11">P11*O11</f>
-        <v>10.251000000000001</v>
+        <v>10.234</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="3"/>
@@ -1889,25 +1898,25 @@
         <v>65</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G12" s="51" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J12" s="10">
-        <v>1924459</v>
+        <v>1868158</v>
       </c>
       <c r="K12" s="46" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="L12" s="42">
         <v>1</v>
@@ -1923,11 +1932,11 @@
         <v>1000</v>
       </c>
       <c r="P12" s="30">
-        <v>9.8899999999999995E-3</v>
+        <v>4.4900000000000001E-3</v>
       </c>
       <c r="Q12" s="30">
         <f>P12*O12</f>
-        <v>9.8899999999999988</v>
+        <v>4.49</v>
       </c>
       <c r="R12" s="48">
         <f>ROW(R12) - ROW($A$1)</f>
@@ -1949,25 +1958,25 @@
         <v>65</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H13" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J13" s="10">
-        <v>23930</v>
+        <v>69395</v>
       </c>
       <c r="K13" s="46" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L13" s="42">
         <v>1</v>
@@ -1983,18 +1992,18 @@
         <v>100</v>
       </c>
       <c r="P13" s="30">
-        <v>3.1469999999999998E-2</v>
+        <v>1.167E-2</v>
       </c>
       <c r="Q13" s="30">
         <f t="shared" ref="Q13" si="13">P13*O13</f>
-        <v>3.1469999999999998</v>
+        <v>1.167</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>ROW(A14) - ROW($A$1)</f>
         <v>13</v>
@@ -2006,28 +2015,28 @@
         <v>48</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H14" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J14" s="10">
-        <v>231704</v>
+        <v>84527</v>
       </c>
       <c r="K14" s="46" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="L14" s="42">
         <v>1</v>
@@ -2043,18 +2052,18 @@
         <v>200</v>
       </c>
       <c r="P14" s="30">
-        <v>1.7979999999999999E-2</v>
+        <v>1.167E-2</v>
       </c>
       <c r="Q14" s="30">
         <f>P14*O14</f>
-        <v>3.5960000000000001</v>
+        <v>2.3340000000000001</v>
       </c>
       <c r="R14" s="48">
         <f>ROW(R14) - ROW($A$1)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2069,25 +2078,25 @@
         <v>65</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H15" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J15" s="10">
-        <v>54524</v>
+        <v>135537</v>
       </c>
       <c r="K15" s="46" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="L15" s="42">
         <v>1</v>
@@ -2103,11 +2112,11 @@
         <v>200</v>
       </c>
       <c r="P15" s="30">
-        <v>2.3380000000000001E-2</v>
+        <v>1.167E-2</v>
       </c>
       <c r="Q15" s="30">
         <f t="shared" ref="Q15:Q17" si="15">P15*O15</f>
-        <v>4.6760000000000002</v>
+        <v>2.3340000000000001</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
@@ -2129,25 +2138,25 @@
         <v>65</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J16" s="10">
-        <v>70706</v>
+        <v>99644</v>
       </c>
       <c r="K16" s="46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="L16" s="42">
         <v>1</v>
@@ -2163,11 +2172,11 @@
         <v>100</v>
       </c>
       <c r="P16" s="30">
-        <v>2.1579999999999998E-2</v>
+        <v>1.167E-2</v>
       </c>
       <c r="Q16" s="30">
         <f>P16*O16</f>
-        <v>2.1579999999999999</v>
+        <v>1.167</v>
       </c>
       <c r="R16" s="48">
         <f>ROW(R16) - ROW($A$1)</f>
@@ -2189,25 +2198,25 @@
         <v>65</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G17" s="51" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J17" s="10">
-        <v>4399293</v>
+        <v>900334</v>
       </c>
       <c r="K17" s="46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="L17" s="42">
         <v>1</v>
@@ -2223,11 +2232,11 @@
         <v>100</v>
       </c>
       <c r="P17" s="30">
-        <v>8.9899999999999997E-3</v>
+        <v>5.3899999999999998E-3</v>
       </c>
       <c r="Q17" s="30">
         <f t="shared" ref="Q17" si="17">P17*O17</f>
-        <v>0.89900000000000002</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="R17" s="48">
         <f t="shared" si="3"/>
@@ -2246,28 +2255,28 @@
         <v>52</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J18" s="10">
-        <v>19360</v>
+        <v>18062</v>
       </c>
       <c r="K18" s="46" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L18" s="42">
         <v>1</v>
@@ -2283,11 +2292,11 @@
         <v>100</v>
       </c>
       <c r="P18" s="30">
-        <v>1.529E-2</v>
+        <v>2.4240000000000001E-2</v>
       </c>
       <c r="Q18" s="30">
         <f>P18*O18</f>
-        <v>1.5289999999999999</v>
+        <v>2.4239999999999999</v>
       </c>
       <c r="R18" s="48">
         <f>ROW(R18) - ROW($A$1)</f>
@@ -2306,28 +2315,28 @@
         <v>53</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G19" s="51" t="s">
         <v>53</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J19" s="10">
         <v>15015</v>
       </c>
       <c r="K19" s="46" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="L19" s="42">
         <v>1</v>
@@ -2343,11 +2352,11 @@
         <v>200</v>
       </c>
       <c r="P19" s="30">
-        <v>0.48826999999999998</v>
+        <v>0.48743999999999998</v>
       </c>
       <c r="Q19" s="30">
         <f t="shared" ref="Q19:Q22" si="19">P19*O19</f>
-        <v>97.653999999999996</v>
+        <v>97.488</v>
       </c>
       <c r="R19" s="48">
         <f t="shared" si="3"/>
@@ -2366,26 +2375,26 @@
         <v>54</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G20" s="51" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H20" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J20" s="10">
         <v>843</v>
       </c>
       <c r="K20" s="46" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="L20" s="42">
         <v>1</v>
@@ -2401,11 +2410,11 @@
         <v>100</v>
       </c>
       <c r="P20" s="30">
-        <v>2.99</v>
+        <v>2.98</v>
       </c>
       <c r="Q20" s="30">
         <f>P20*O20</f>
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R20" s="48">
         <f>ROW(R20) - ROW($A$1)</f>
@@ -2424,26 +2433,26 @@
         <v>55</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="51" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G21" s="51" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H21" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J21" s="10">
         <v>27461</v>
       </c>
       <c r="K21" s="46" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L21" s="42">
         <v>1</v>
@@ -2459,11 +2468,11 @@
         <v>100</v>
       </c>
       <c r="P21" s="30">
-        <v>0.38845000000000002</v>
+        <v>0.38779999999999998</v>
       </c>
       <c r="Q21" s="30">
         <f t="shared" ref="Q21" si="21">P21*O21</f>
-        <v>38.844999999999999</v>
+        <v>38.78</v>
       </c>
       <c r="R21" s="48">
         <f t="shared" si="3"/>
@@ -2482,28 +2491,28 @@
         <v>56</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H22" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J22" s="10">
-        <v>959</v>
+        <v>930</v>
       </c>
       <c r="K22" s="46" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L22" s="42">
         <v>1</v>
@@ -2519,11 +2528,11 @@
         <v>100</v>
       </c>
       <c r="P22" s="30">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="Q22" s="30">
         <f>P22*O22</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R22" s="48">
         <f>ROW(R22) - ROW($A$1)</f>
@@ -2570,7 +2579,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="34">
         <f ca="1">NOW()</f>
-        <v>43843.738721527778</v>
+        <v>43844.492883564817</v>
       </c>
       <c r="L24" s="40"/>
       <c r="M24" s="15"/>
@@ -2581,11 +2590,11 @@
       </c>
       <c r="Q24" s="36">
         <f>SUM(Q2:Q22)</f>
-        <v>752.05489999999998</v>
+        <v>689.23360000000002</v>
       </c>
       <c r="R24" s="50">
         <f>Q24/N25</f>
-        <v>37.602744999999999</v>
+        <v>34.461680000000001</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update pcb and submit pcb file to betalayout
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\n-blocks\n-dap\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B86B0947-896A-4A64-BE67-9B4E09066D6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6A3C2BD-9556-4682-9B67-12CC6E4F9D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseList" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>11:31</t>
+    <t>16:31</t>
   </si>
   <si>
     <t>36</t>
@@ -1321,7 +1321,7 @@
         <v>116</v>
       </c>
       <c r="J2" s="10">
-        <v>40946</v>
+        <v>37050</v>
       </c>
       <c r="K2" s="46" t="s">
         <v>119</v>
@@ -1340,11 +1340,11 @@
         <v>108</v>
       </c>
       <c r="P2" s="30">
-        <v>1.8870000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="Q2" s="30">
         <f>P2*O2</f>
-        <v>2.03796</v>
+        <v>2.052</v>
       </c>
       <c r="R2" s="48">
         <f>ROW(R2) - ROW($A$1)</f>
@@ -1400,11 +1400,11 @@
         <v>100</v>
       </c>
       <c r="P3" s="30">
-        <v>3.594E-2</v>
+        <v>3.6200000000000003E-2</v>
       </c>
       <c r="Q3" s="30">
         <f t="shared" ref="Q3:Q22" si="2">P3*O3</f>
-        <v>3.5939999999999999</v>
+        <v>3.62</v>
       </c>
       <c r="R3" s="48">
         <f t="shared" ref="R3:R22" si="3">ROW(R3) - ROW($A$1)</f>
@@ -1441,7 +1441,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="10">
-        <v>34052</v>
+        <v>33872</v>
       </c>
       <c r="K4" s="46" t="s">
         <v>121</v>
@@ -1460,11 +1460,11 @@
         <v>72</v>
       </c>
       <c r="P4" s="30">
-        <v>1.4370000000000001E-2</v>
+        <v>1.448E-2</v>
       </c>
       <c r="Q4" s="30">
         <f>P4*O4</f>
-        <v>1.03464</v>
+        <v>1.0425599999999999</v>
       </c>
       <c r="R4" s="48">
         <f>ROW(R4) - ROW($A$1)</f>
@@ -1501,7 +1501,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="10">
-        <v>25442</v>
+        <v>9999</v>
       </c>
       <c r="K5" s="46" t="s">
         <v>122</v>
@@ -1520,11 +1520,11 @@
         <v>100</v>
       </c>
       <c r="P5" s="30">
-        <v>2.8750000000000001E-2</v>
+        <v>2.896E-2</v>
       </c>
       <c r="Q5" s="30">
         <f t="shared" ref="Q5" si="5">P5*O5</f>
-        <v>2.875</v>
+        <v>2.8959999999999999</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="3"/>
@@ -1559,7 +1559,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="10">
-        <v>67675</v>
+        <v>59043</v>
       </c>
       <c r="K6" s="46" t="s">
         <v>123</v>
@@ -1578,11 +1578,11 @@
         <v>100</v>
       </c>
       <c r="P6" s="30">
-        <v>6.8279999999999993E-2</v>
+        <v>6.8769999999999998E-2</v>
       </c>
       <c r="Q6" s="30">
         <f>P6*O6</f>
-        <v>6.8279999999999994</v>
+        <v>6.8769999999999998</v>
       </c>
       <c r="R6" s="48">
         <f>ROW(R6) - ROW($A$1)</f>
@@ -1617,7 +1617,7 @@
         <v>116</v>
       </c>
       <c r="J7" s="10">
-        <v>40404</v>
+        <v>98272</v>
       </c>
       <c r="K7" s="46" t="s">
         <v>124</v>
@@ -1636,11 +1636,11 @@
         <v>36</v>
       </c>
       <c r="P7" s="30">
-        <v>0.10421</v>
+        <v>0.10496999999999999</v>
       </c>
       <c r="Q7" s="30">
         <f t="shared" ref="Q7:Q9" si="7">P7*O7</f>
-        <v>3.75156</v>
+        <v>3.7789199999999998</v>
       </c>
       <c r="R7" s="48">
         <f t="shared" si="3"/>
@@ -1675,7 +1675,7 @@
         <v>116</v>
       </c>
       <c r="J8" s="10">
-        <v>58553</v>
+        <v>57880</v>
       </c>
       <c r="K8" s="46" t="s">
         <v>125</v>
@@ -1694,11 +1694,11 @@
         <v>36</v>
       </c>
       <c r="P8" s="30">
-        <v>0.26951999999999998</v>
+        <v>0.27146999999999999</v>
       </c>
       <c r="Q8" s="30">
         <f>P8*O8</f>
-        <v>9.7027199999999993</v>
+        <v>9.7729199999999992</v>
       </c>
       <c r="R8" s="48">
         <f>ROW(R8) - ROW($A$1)</f>
@@ -1735,7 +1735,7 @@
         <v>116</v>
       </c>
       <c r="J9" s="10">
-        <v>115642</v>
+        <v>116092</v>
       </c>
       <c r="K9" s="46" t="s">
         <v>126</v>
@@ -1754,11 +1754,11 @@
         <v>47</v>
       </c>
       <c r="P9" s="30">
-        <v>0.34227999999999997</v>
+        <v>0.34477000000000002</v>
       </c>
       <c r="Q9" s="30">
         <f t="shared" ref="Q9" si="9">P9*O9</f>
-        <v>16.087159999999997</v>
+        <v>16.204190000000001</v>
       </c>
       <c r="R9" s="48">
         <f t="shared" si="3"/>
@@ -1793,7 +1793,7 @@
         <v>116</v>
       </c>
       <c r="J10" s="10">
-        <v>21413</v>
+        <v>21003</v>
       </c>
       <c r="K10" s="46" t="s">
         <v>127</v>
@@ -1812,11 +1812,11 @@
         <v>36</v>
       </c>
       <c r="P10" s="30">
-        <v>0.66839999999999999</v>
+        <v>0.67325000000000002</v>
       </c>
       <c r="Q10" s="30">
         <f>P10*O10</f>
-        <v>24.0624</v>
+        <v>24.237000000000002</v>
       </c>
       <c r="R10" s="48">
         <f>ROW(R10) - ROW($A$1)</f>
@@ -1853,7 +1853,7 @@
         <v>116</v>
       </c>
       <c r="J11" s="10">
-        <v>97989</v>
+        <v>94764</v>
       </c>
       <c r="K11" s="46" t="s">
         <v>128</v>
@@ -1872,11 +1872,11 @@
         <v>36</v>
       </c>
       <c r="P11" s="30">
-        <v>0.23896999999999999</v>
+        <v>0.2407</v>
       </c>
       <c r="Q11" s="30">
         <f t="shared" ref="Q11:Q17" si="11">P11*O11</f>
-        <v>8.6029199999999992</v>
+        <v>8.6652000000000005</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="3"/>
@@ -1913,7 +1913,7 @@
         <v>116</v>
       </c>
       <c r="J12" s="10">
-        <v>1859432</v>
+        <v>1836811</v>
       </c>
       <c r="K12" s="46" t="s">
         <v>129</v>
@@ -1932,11 +1932,11 @@
         <v>180</v>
       </c>
       <c r="P12" s="30">
-        <v>1.1679999999999999E-2</v>
+        <v>1.176E-2</v>
       </c>
       <c r="Q12" s="30">
         <f>P12*O12</f>
-        <v>2.1023999999999998</v>
+        <v>2.1168</v>
       </c>
       <c r="R12" s="48">
         <f>ROW(R12) - ROW($A$1)</f>
@@ -1973,7 +1973,7 @@
         <v>116</v>
       </c>
       <c r="J13" s="10">
-        <v>69395</v>
+        <v>68380</v>
       </c>
       <c r="K13" s="46" t="s">
         <v>130</v>
@@ -1992,11 +1992,11 @@
         <v>36</v>
       </c>
       <c r="P13" s="30">
-        <v>2.8750000000000001E-2</v>
+        <v>2.896E-2</v>
       </c>
       <c r="Q13" s="30">
         <f t="shared" ref="Q13" si="13">P13*O13</f>
-        <v>1.0350000000000001</v>
+        <v>1.0425599999999999</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="3"/>
@@ -2033,7 +2033,7 @@
         <v>116</v>
       </c>
       <c r="J14" s="10">
-        <v>84497</v>
+        <v>83930</v>
       </c>
       <c r="K14" s="46" t="s">
         <v>131</v>
@@ -2052,11 +2052,11 @@
         <v>100</v>
       </c>
       <c r="P14" s="30">
-        <v>1.1679999999999999E-2</v>
+        <v>1.176E-2</v>
       </c>
       <c r="Q14" s="30">
         <f>P14*O14</f>
-        <v>1.1679999999999999</v>
+        <v>1.1759999999999999</v>
       </c>
       <c r="R14" s="48">
         <f>ROW(R14) - ROW($A$1)</f>
@@ -2093,7 +2093,7 @@
         <v>116</v>
       </c>
       <c r="J15" s="10">
-        <v>135522</v>
+        <v>131942</v>
       </c>
       <c r="K15" s="46" t="s">
         <v>132</v>
@@ -2112,11 +2112,11 @@
         <v>100</v>
       </c>
       <c r="P15" s="30">
-        <v>1.1679999999999999E-2</v>
+        <v>1.176E-2</v>
       </c>
       <c r="Q15" s="30">
         <f t="shared" ref="Q15:Q17" si="15">P15*O15</f>
-        <v>1.1679999999999999</v>
+        <v>1.1759999999999999</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
@@ -2153,7 +2153,7 @@
         <v>116</v>
       </c>
       <c r="J16" s="10">
-        <v>99619</v>
+        <v>98927</v>
       </c>
       <c r="K16" s="46" t="s">
         <v>133</v>
@@ -2172,11 +2172,11 @@
         <v>36</v>
       </c>
       <c r="P16" s="30">
-        <v>2.8750000000000001E-2</v>
+        <v>2.896E-2</v>
       </c>
       <c r="Q16" s="30">
         <f>P16*O16</f>
-        <v>1.0350000000000001</v>
+        <v>1.0425599999999999</v>
       </c>
       <c r="R16" s="48">
         <f>ROW(R16) - ROW($A$1)</f>
@@ -2213,7 +2213,7 @@
         <v>116</v>
       </c>
       <c r="J17" s="10">
-        <v>899812</v>
+        <v>891522</v>
       </c>
       <c r="K17" s="46" t="s">
         <v>134</v>
@@ -2232,11 +2232,11 @@
         <v>36</v>
       </c>
       <c r="P17" s="30">
-        <v>1.4370000000000001E-2</v>
+        <v>1.448E-2</v>
       </c>
       <c r="Q17" s="30">
         <f t="shared" ref="Q17" si="17">P17*O17</f>
-        <v>0.51732</v>
+        <v>0.52127999999999997</v>
       </c>
       <c r="R17" s="48">
         <f t="shared" si="3"/>
@@ -2273,7 +2273,7 @@
         <v>116</v>
       </c>
       <c r="J18" s="10">
-        <v>17512</v>
+        <v>16412</v>
       </c>
       <c r="K18" s="46" t="s">
         <v>135</v>
@@ -2292,11 +2292,11 @@
         <v>36</v>
       </c>
       <c r="P18" s="30">
-        <v>3.5040000000000002E-2</v>
+        <v>3.5290000000000002E-2</v>
       </c>
       <c r="Q18" s="30">
         <f>P18*O18</f>
-        <v>1.2614400000000001</v>
+        <v>1.27044</v>
       </c>
       <c r="R18" s="48">
         <f>ROW(R18) - ROW($A$1)</f>
@@ -2333,7 +2333,7 @@
         <v>116</v>
       </c>
       <c r="J19" s="10">
-        <v>15015</v>
+        <v>14994</v>
       </c>
       <c r="K19" s="46" t="s">
         <v>136</v>
@@ -2352,11 +2352,11 @@
         <v>72</v>
       </c>
       <c r="P19" s="30">
-        <v>0.64773000000000003</v>
+        <v>0.65244000000000002</v>
       </c>
       <c r="Q19" s="30">
         <f t="shared" ref="Q19:Q22" si="19">P19*O19</f>
-        <v>46.636560000000003</v>
+        <v>46.975680000000004</v>
       </c>
       <c r="R19" s="48">
         <f t="shared" si="3"/>
@@ -2410,11 +2410,11 @@
         <v>36</v>
       </c>
       <c r="P20" s="30">
-        <v>3.44</v>
+        <v>3.47</v>
       </c>
       <c r="Q20" s="30">
         <f>P20*O20</f>
-        <v>123.84</v>
+        <v>124.92</v>
       </c>
       <c r="R20" s="48">
         <f>ROW(R20) - ROW($A$1)</f>
@@ -2449,7 +2449,7 @@
         <v>116</v>
       </c>
       <c r="J21" s="10">
-        <v>27457</v>
+        <v>27364</v>
       </c>
       <c r="K21" s="46" t="s">
         <v>138</v>
@@ -2468,11 +2468,11 @@
         <v>36</v>
       </c>
       <c r="P21" s="30">
-        <v>0.60192000000000001</v>
+        <v>0.60629</v>
       </c>
       <c r="Q21" s="30">
         <f t="shared" ref="Q21" si="21">P21*O21</f>
-        <v>21.669119999999999</v>
+        <v>21.826439999999998</v>
       </c>
       <c r="R21" s="48">
         <f t="shared" si="3"/>
@@ -2509,7 +2509,7 @@
         <v>116</v>
       </c>
       <c r="J22" s="10">
-        <v>930</v>
+        <v>530</v>
       </c>
       <c r="K22" s="46" t="s">
         <v>139</v>
@@ -2528,11 +2528,11 @@
         <v>36</v>
       </c>
       <c r="P22" s="30">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="Q22" s="30">
         <f>P22*O22</f>
-        <v>43.92</v>
+        <v>44.28</v>
       </c>
       <c r="R22" s="48">
         <f>ROW(R22) - ROW($A$1)</f>
@@ -2579,7 +2579,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="34">
         <f ca="1">NOW()</f>
-        <v>43845.480064467592</v>
+        <v>43854.688447569446</v>
       </c>
       <c r="L24" s="40"/>
       <c r="M24" s="15"/>
@@ -2590,11 +2590,11 @@
       </c>
       <c r="Q24" s="36">
         <f>SUM(Q2:Q22)</f>
-        <v>322.92920000000004</v>
+        <v>325.49355000000003</v>
       </c>
       <c r="R24" s="50">
         <f>Q24/N25</f>
-        <v>8.970255555555557</v>
+        <v>9.0414875000000006</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
assembly file for betalayout
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\n-blocks\n-dap\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6A3C2BD-9556-4682-9B67-12CC6E4F9D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75928E3E-76B0-4E90-B460-74A522EABA82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseList" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <t>n-DAP</t>
   </si>
   <si>
-    <t>16:31</t>
+    <t>21:05</t>
   </si>
   <si>
     <t>36</t>
@@ -1235,7 +1235,7 @@
     <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>116</v>
       </c>
       <c r="J2" s="10">
-        <v>37050</v>
+        <v>14550</v>
       </c>
       <c r="K2" s="46" t="s">
         <v>119</v>
@@ -1340,11 +1340,11 @@
         <v>108</v>
       </c>
       <c r="P2" s="30">
-        <v>1.9E-2</v>
+        <v>1.9050000000000001E-2</v>
       </c>
       <c r="Q2" s="30">
         <f>P2*O2</f>
-        <v>2.052</v>
+        <v>2.0573999999999999</v>
       </c>
       <c r="R2" s="48">
         <f>ROW(R2) - ROW($A$1)</f>
@@ -1381,7 +1381,7 @@
         <v>116</v>
       </c>
       <c r="J3" s="10">
-        <v>5900</v>
+        <v>5760</v>
       </c>
       <c r="K3" s="46" t="s">
         <v>120</v>
@@ -1400,11 +1400,11 @@
         <v>100</v>
       </c>
       <c r="P3" s="30">
-        <v>3.6200000000000003E-2</v>
+        <v>3.628E-2</v>
       </c>
       <c r="Q3" s="30">
         <f t="shared" ref="Q3:Q22" si="2">P3*O3</f>
-        <v>3.62</v>
+        <v>3.6280000000000001</v>
       </c>
       <c r="R3" s="48">
         <f t="shared" ref="R3:R22" si="3">ROW(R3) - ROW($A$1)</f>
@@ -1441,7 +1441,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="10">
-        <v>33872</v>
+        <v>33732</v>
       </c>
       <c r="K4" s="46" t="s">
         <v>121</v>
@@ -1460,11 +1460,11 @@
         <v>72</v>
       </c>
       <c r="P4" s="30">
-        <v>1.448E-2</v>
+        <v>1.451E-2</v>
       </c>
       <c r="Q4" s="30">
         <f>P4*O4</f>
-        <v>1.0425599999999999</v>
+        <v>1.0447200000000001</v>
       </c>
       <c r="R4" s="48">
         <f>ROW(R4) - ROW($A$1)</f>
@@ -1501,7 +1501,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="10">
-        <v>9999</v>
+        <v>9007</v>
       </c>
       <c r="K5" s="46" t="s">
         <v>122</v>
@@ -1520,11 +1520,11 @@
         <v>100</v>
       </c>
       <c r="P5" s="30">
-        <v>2.896E-2</v>
+        <v>2.9020000000000001E-2</v>
       </c>
       <c r="Q5" s="30">
         <f t="shared" ref="Q5" si="5">P5*O5</f>
-        <v>2.8959999999999999</v>
+        <v>2.9020000000000001</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="3"/>
@@ -1559,7 +1559,7 @@
         <v>116</v>
       </c>
       <c r="J6" s="10">
-        <v>59043</v>
+        <v>55905</v>
       </c>
       <c r="K6" s="46" t="s">
         <v>123</v>
@@ -1578,11 +1578,11 @@
         <v>100</v>
       </c>
       <c r="P6" s="30">
-        <v>6.8769999999999998E-2</v>
+        <v>6.8930000000000005E-2</v>
       </c>
       <c r="Q6" s="30">
         <f>P6*O6</f>
-        <v>6.8769999999999998</v>
+        <v>6.8930000000000007</v>
       </c>
       <c r="R6" s="48">
         <f>ROW(R6) - ROW($A$1)</f>
@@ -1617,7 +1617,7 @@
         <v>116</v>
       </c>
       <c r="J7" s="10">
-        <v>98272</v>
+        <v>85016</v>
       </c>
       <c r="K7" s="46" t="s">
         <v>124</v>
@@ -1636,11 +1636,11 @@
         <v>36</v>
       </c>
       <c r="P7" s="30">
-        <v>0.10496999999999999</v>
+        <v>0.10521</v>
       </c>
       <c r="Q7" s="30">
         <f t="shared" ref="Q7:Q9" si="7">P7*O7</f>
-        <v>3.7789199999999998</v>
+        <v>3.78756</v>
       </c>
       <c r="R7" s="48">
         <f t="shared" si="3"/>
@@ -1675,7 +1675,7 @@
         <v>116</v>
       </c>
       <c r="J8" s="10">
-        <v>57880</v>
+        <v>57670</v>
       </c>
       <c r="K8" s="46" t="s">
         <v>125</v>
@@ -1694,11 +1694,11 @@
         <v>36</v>
       </c>
       <c r="P8" s="30">
-        <v>0.27146999999999999</v>
+        <v>0.27210000000000001</v>
       </c>
       <c r="Q8" s="30">
         <f>P8*O8</f>
-        <v>9.7729199999999992</v>
+        <v>9.7956000000000003</v>
       </c>
       <c r="R8" s="48">
         <f>ROW(R8) - ROW($A$1)</f>
@@ -1735,7 +1735,7 @@
         <v>116</v>
       </c>
       <c r="J9" s="10">
-        <v>116092</v>
+        <v>112788</v>
       </c>
       <c r="K9" s="46" t="s">
         <v>126</v>
@@ -1754,11 +1754,11 @@
         <v>47</v>
       </c>
       <c r="P9" s="30">
-        <v>0.34477000000000002</v>
+        <v>0.34556999999999999</v>
       </c>
       <c r="Q9" s="30">
         <f t="shared" ref="Q9" si="9">P9*O9</f>
-        <v>16.204190000000001</v>
+        <v>16.241789999999998</v>
       </c>
       <c r="R9" s="48">
         <f t="shared" si="3"/>
@@ -1793,7 +1793,7 @@
         <v>116</v>
       </c>
       <c r="J10" s="10">
-        <v>21003</v>
+        <v>18449</v>
       </c>
       <c r="K10" s="46" t="s">
         <v>127</v>
@@ -1812,11 +1812,11 @@
         <v>36</v>
       </c>
       <c r="P10" s="30">
-        <v>0.67325000000000002</v>
+        <v>0.67481000000000002</v>
       </c>
       <c r="Q10" s="30">
         <f>P10*O10</f>
-        <v>24.237000000000002</v>
+        <v>24.29316</v>
       </c>
       <c r="R10" s="48">
         <f>ROW(R10) - ROW($A$1)</f>
@@ -1853,7 +1853,7 @@
         <v>116</v>
       </c>
       <c r="J11" s="10">
-        <v>94764</v>
+        <v>94693</v>
       </c>
       <c r="K11" s="46" t="s">
         <v>128</v>
@@ -1872,11 +1872,11 @@
         <v>36</v>
       </c>
       <c r="P11" s="30">
-        <v>0.2407</v>
+        <v>0.24126</v>
       </c>
       <c r="Q11" s="30">
         <f t="shared" ref="Q11:Q17" si="11">P11*O11</f>
-        <v>8.6652000000000005</v>
+        <v>8.6853599999999993</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="3"/>
@@ -1913,7 +1913,7 @@
         <v>116</v>
       </c>
       <c r="J12" s="10">
-        <v>1836811</v>
+        <v>1804342</v>
       </c>
       <c r="K12" s="46" t="s">
         <v>129</v>
@@ -1932,11 +1932,11 @@
         <v>180</v>
       </c>
       <c r="P12" s="30">
-        <v>1.176E-2</v>
+        <v>1.179E-2</v>
       </c>
       <c r="Q12" s="30">
         <f>P12*O12</f>
-        <v>2.1168</v>
+        <v>2.1221999999999999</v>
       </c>
       <c r="R12" s="48">
         <f>ROW(R12) - ROW($A$1)</f>
@@ -1973,7 +1973,7 @@
         <v>116</v>
       </c>
       <c r="J13" s="10">
-        <v>68380</v>
+        <v>68280</v>
       </c>
       <c r="K13" s="46" t="s">
         <v>130</v>
@@ -1992,11 +1992,11 @@
         <v>36</v>
       </c>
       <c r="P13" s="30">
-        <v>2.896E-2</v>
+        <v>2.9020000000000001E-2</v>
       </c>
       <c r="Q13" s="30">
         <f t="shared" ref="Q13" si="13">P13*O13</f>
-        <v>1.0425599999999999</v>
+        <v>1.0447200000000001</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="3"/>
@@ -2033,7 +2033,7 @@
         <v>116</v>
       </c>
       <c r="J14" s="10">
-        <v>83930</v>
+        <v>83450</v>
       </c>
       <c r="K14" s="46" t="s">
         <v>131</v>
@@ -2052,11 +2052,11 @@
         <v>100</v>
       </c>
       <c r="P14" s="30">
-        <v>1.176E-2</v>
+        <v>1.179E-2</v>
       </c>
       <c r="Q14" s="30">
         <f>P14*O14</f>
-        <v>1.1759999999999999</v>
+        <v>1.179</v>
       </c>
       <c r="R14" s="48">
         <f>ROW(R14) - ROW($A$1)</f>
@@ -2093,7 +2093,7 @@
         <v>116</v>
       </c>
       <c r="J15" s="10">
-        <v>131942</v>
+        <v>131140</v>
       </c>
       <c r="K15" s="46" t="s">
         <v>132</v>
@@ -2112,11 +2112,11 @@
         <v>100</v>
       </c>
       <c r="P15" s="30">
-        <v>1.176E-2</v>
+        <v>1.179E-2</v>
       </c>
       <c r="Q15" s="30">
         <f t="shared" ref="Q15:Q17" si="15">P15*O15</f>
-        <v>1.1759999999999999</v>
+        <v>1.179</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
@@ -2153,7 +2153,7 @@
         <v>116</v>
       </c>
       <c r="J16" s="10">
-        <v>98927</v>
+        <v>88605</v>
       </c>
       <c r="K16" s="46" t="s">
         <v>133</v>
@@ -2172,11 +2172,11 @@
         <v>36</v>
       </c>
       <c r="P16" s="30">
-        <v>2.896E-2</v>
+        <v>2.9020000000000001E-2</v>
       </c>
       <c r="Q16" s="30">
         <f>P16*O16</f>
-        <v>1.0425599999999999</v>
+        <v>1.0447200000000001</v>
       </c>
       <c r="R16" s="48">
         <f>ROW(R16) - ROW($A$1)</f>
@@ -2213,7 +2213,7 @@
         <v>116</v>
       </c>
       <c r="J17" s="10">
-        <v>891522</v>
+        <v>857327</v>
       </c>
       <c r="K17" s="46" t="s">
         <v>134</v>
@@ -2232,11 +2232,11 @@
         <v>36</v>
       </c>
       <c r="P17" s="30">
-        <v>1.448E-2</v>
+        <v>1.451E-2</v>
       </c>
       <c r="Q17" s="30">
         <f t="shared" ref="Q17" si="17">P17*O17</f>
-        <v>0.52127999999999997</v>
+        <v>0.52236000000000005</v>
       </c>
       <c r="R17" s="48">
         <f t="shared" si="3"/>
@@ -2273,7 +2273,7 @@
         <v>116</v>
       </c>
       <c r="J18" s="10">
-        <v>16412</v>
+        <v>16077</v>
       </c>
       <c r="K18" s="46" t="s">
         <v>135</v>
@@ -2292,11 +2292,11 @@
         <v>36</v>
       </c>
       <c r="P18" s="30">
-        <v>3.5290000000000002E-2</v>
+        <v>3.5369999999999999E-2</v>
       </c>
       <c r="Q18" s="30">
         <f>P18*O18</f>
-        <v>1.27044</v>
+        <v>1.27332</v>
       </c>
       <c r="R18" s="48">
         <f>ROW(R18) - ROW($A$1)</f>
@@ -2333,7 +2333,7 @@
         <v>116</v>
       </c>
       <c r="J19" s="10">
-        <v>14994</v>
+        <v>14899</v>
       </c>
       <c r="K19" s="46" t="s">
         <v>136</v>
@@ -2352,11 +2352,11 @@
         <v>72</v>
       </c>
       <c r="P19" s="30">
-        <v>0.65244000000000002</v>
+        <v>0.65395000000000003</v>
       </c>
       <c r="Q19" s="30">
         <f t="shared" ref="Q19:Q22" si="19">P19*O19</f>
-        <v>46.975680000000004</v>
+        <v>47.084400000000002</v>
       </c>
       <c r="R19" s="48">
         <f t="shared" si="3"/>
@@ -2391,7 +2391,7 @@
         <v>116</v>
       </c>
       <c r="J20" s="10">
-        <v>843</v>
+        <v>806</v>
       </c>
       <c r="K20" s="46" t="s">
         <v>137</v>
@@ -2449,7 +2449,7 @@
         <v>116</v>
       </c>
       <c r="J21" s="10">
-        <v>27364</v>
+        <v>27275</v>
       </c>
       <c r="K21" s="46" t="s">
         <v>138</v>
@@ -2468,11 +2468,11 @@
         <v>36</v>
       </c>
       <c r="P21" s="30">
-        <v>0.60629</v>
+        <v>0.60768999999999995</v>
       </c>
       <c r="Q21" s="30">
         <f t="shared" ref="Q21" si="21">P21*O21</f>
-        <v>21.826439999999998</v>
+        <v>21.876839999999998</v>
       </c>
       <c r="R21" s="48">
         <f t="shared" si="3"/>
@@ -2509,7 +2509,7 @@
         <v>116</v>
       </c>
       <c r="J22" s="10">
-        <v>530</v>
+        <v>478</v>
       </c>
       <c r="K22" s="46" t="s">
         <v>139</v>
@@ -2579,7 +2579,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="34">
         <f ca="1">NOW()</f>
-        <v>43854.688447569446</v>
+        <v>43860.878761689812</v>
       </c>
       <c r="L24" s="40"/>
       <c r="M24" s="15"/>
@@ -2590,11 +2590,11 @@
       </c>
       <c r="Q24" s="36">
         <f>SUM(Q2:Q22)</f>
-        <v>325.49355000000003</v>
+        <v>325.85515000000009</v>
       </c>
       <c r="R24" s="50">
         <f>Q24/N25</f>
-        <v>9.0414875000000006</v>
+        <v>9.0515319444444469</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>